<commit_message>
Save for no rage bait
</commit_message>
<xml_diff>
--- a/Bill of Materials (version 1).xlsx
+++ b/Bill of Materials (version 1).xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruijs\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruijs\Desktop\ETEME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{130211CC-B21B-42B6-B34B-9E7E35A08FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A7CBF4-0857-4512-8812-EEC0C533DDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4392" yWindow="828" windowWidth="21504" windowHeight="11040" xr2:uid="{2E597B4C-CD0B-46B8-B788-655E1D3EBACE}"/>
+    <workbookView xWindow="240" yWindow="1620" windowWidth="21504" windowHeight="11040" xr2:uid="{2E597B4C-CD0B-46B8-B788-655E1D3EBACE}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="Cálculos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -342,9 +341,6 @@
     <t>Custo Unitário</t>
   </si>
   <si>
-    <t>Fios de Aço</t>
-  </si>
-  <si>
     <t>kg/m^3</t>
   </si>
   <si>
@@ -409,6 +405,9 @@
   </si>
   <si>
     <t>302,35 + 357,49 + 2,50= 662,34</t>
+  </si>
+  <si>
+    <t>Fio de Aço</t>
   </si>
 </sst>
 </file>
@@ -1323,6 +1322,123 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="42" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1343,123 +1459,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="42" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1873,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5183EBD1-9A1E-4780-80A8-7EF58E7B615D}">
   <dimension ref="B2:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="99" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21:I21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="93" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1898,21 +1897,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="65.25" customHeight="1" x14ac:dyDescent="1.2">
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="126"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="10"/>
@@ -1924,22 +1923,22 @@
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="99" t="s">
+      <c r="F4" s="138" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="100"/>
+      <c r="G4" s="139"/>
       <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="99" t="s">
+      <c r="I4" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="101"/>
+      <c r="J4" s="140"/>
       <c r="K4" s="4" t="s">
         <v>31</v>
       </c>
@@ -2013,7 +2012,7 @@
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
       <c r="C7" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="74"/>
       <c r="E7" s="74" t="s">
@@ -2032,7 +2031,7 @@
         <v>357.49</v>
       </c>
       <c r="J7" s="70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K7" s="77">
         <f>$I$7</f>
@@ -2044,31 +2043,31 @@
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
       <c r="C8" s="6" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D8" s="74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="74">
         <f>$K$5</f>
         <v>32.063200000000002</v>
       </c>
       <c r="F8" s="85">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G8" s="70" t="s">
         <v>58</v>
       </c>
       <c r="H8" s="74">
-        <v>9.67</v>
-      </c>
-      <c r="I8" s="95" t="s">
+        <v>27.34</v>
+      </c>
+      <c r="I8" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="96"/>
+      <c r="J8" s="135"/>
       <c r="K8" s="77">
         <f>E8*F8+H8</f>
-        <v>234.11240000000001</v>
+        <v>59.403199999999998</v>
       </c>
       <c r="M8" s="60"/>
       <c r="N8" s="16"/>
@@ -2079,14 +2078,14 @@
         <v>3</v>
       </c>
       <c r="D9" s="74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E9" s="74">
         <f>K8</f>
-        <v>234.11240000000001</v>
+        <v>59.403199999999998</v>
       </c>
       <c r="F9" s="85">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G9" s="70" t="s">
         <v>58</v>
@@ -2094,13 +2093,13 @@
       <c r="H9" s="74">
         <v>4</v>
       </c>
-      <c r="I9" s="95" t="s">
+      <c r="I9" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="96"/>
+      <c r="J9" s="135"/>
       <c r="K9" s="77">
         <f>E9*F9+H9</f>
-        <v>238.11240000000001</v>
+        <v>419.82240000000002</v>
       </c>
       <c r="M9" s="60"/>
       <c r="N9" s="11"/>
@@ -2111,11 +2110,11 @@
         <v>4</v>
       </c>
       <c r="D10" s="74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="74">
         <f>K9</f>
-        <v>238.11240000000001</v>
+        <v>419.82240000000002</v>
       </c>
       <c r="F10" s="85">
         <v>1</v>
@@ -2126,13 +2125,13 @@
       <c r="H10" s="74">
         <v>1.02</v>
       </c>
-      <c r="I10" s="95" t="s">
+      <c r="I10" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="96"/>
+      <c r="J10" s="135"/>
       <c r="K10" s="77">
         <f>E10*F10+H10</f>
-        <v>239.13240000000002</v>
+        <v>420.8424</v>
       </c>
       <c r="M10" s="60"/>
       <c r="N10" s="11"/>
@@ -2140,14 +2139,14 @@
     <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
       <c r="C11" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="75">
         <f>K10</f>
-        <v>239.13240000000002</v>
+        <v>420.8424</v>
       </c>
       <c r="F11" s="86">
         <f>ROUNDDOWN(Cálculos!E12,0)</f>
@@ -2159,13 +2158,13 @@
       <c r="H11" s="75">
         <v>2.5</v>
       </c>
-      <c r="I11" s="97" t="s">
+      <c r="I11" s="136" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="98"/>
+      <c r="J11" s="137"/>
       <c r="K11" s="78">
         <f>E11*F11+H11</f>
-        <v>5024.2804000000006</v>
+        <v>8840.1903999999995</v>
       </c>
       <c r="N11" s="11"/>
     </row>
@@ -2179,19 +2178,19 @@
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
-      <c r="C14" s="102" t="s">
+      <c r="C14" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="103"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="104"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116"/>
+      <c r="K14" s="116"/>
+      <c r="L14" s="116"/>
+      <c r="M14" s="103"/>
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2202,20 +2201,20 @@
       <c r="D15" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="136" t="s">
+      <c r="E15" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="137"/>
-      <c r="G15" s="119" t="s">
+      <c r="F15" s="111"/>
+      <c r="G15" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="119"/>
-      <c r="I15" s="119"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="136" t="s">
+      <c r="H15" s="129"/>
+      <c r="I15" s="129"/>
+      <c r="J15" s="129"/>
+      <c r="K15" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="137"/>
+      <c r="L15" s="111"/>
       <c r="M15" s="84" t="s">
         <v>9</v>
       </c>
@@ -2227,20 +2226,20 @@
         <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" s="87">
         <v>520</v>
       </c>
       <c r="F16" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="120" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
-      <c r="J16" s="120"/>
+      <c r="H16" s="130"/>
+      <c r="I16" s="130"/>
+      <c r="J16" s="130"/>
       <c r="K16" s="67">
         <v>61.65</v>
       </c>
@@ -2259,20 +2258,20 @@
         <v>2</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="61">
         <v>2340.3200000000002</v>
       </c>
       <c r="F17" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="131"/>
+      <c r="J17" s="131"/>
       <c r="K17" s="61">
         <v>2.2400000000000002</v>
       </c>
@@ -2288,23 +2287,23 @@
     <row r="18" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="10"/>
       <c r="C18" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E18" s="61">
         <v>357.49</v>
       </c>
       <c r="F18" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="131" t="s">
         <v>104</v>
       </c>
-      <c r="G18" s="121" t="s">
-        <v>105</v>
-      </c>
-      <c r="H18" s="121"/>
-      <c r="I18" s="121"/>
-      <c r="J18" s="121"/>
+      <c r="H18" s="131"/>
+      <c r="I18" s="131"/>
+      <c r="J18" s="131"/>
       <c r="K18" s="61">
         <v>1</v>
       </c>
@@ -2332,15 +2331,15 @@
       <c r="D21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="131" t="s">
+      <c r="E21" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="104"/>
-      <c r="G21" s="138" t="s">
+      <c r="F21" s="103"/>
+      <c r="G21" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="139"/>
-      <c r="I21" s="140"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="114"/>
       <c r="N21" s="11"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
@@ -2349,45 +2348,45 @@
         <v>22</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="132">
+      <c r="E22" s="104">
         <v>1000</v>
       </c>
-      <c r="F22" s="133"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="117"/>
-      <c r="I22" s="118"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="128"/>
       <c r="N22" s="11"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
-      <c r="C23" s="127" t="s">
+      <c r="C23" s="98" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="111">
+      <c r="E23" s="123">
         <v>17590</v>
       </c>
-      <c r="F23" s="112"/>
-      <c r="G23" s="107" t="s">
+      <c r="F23" s="124"/>
+      <c r="G23" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="107"/>
-      <c r="I23" s="108"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="120"/>
       <c r="N23" s="11"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="10"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="101"/>
       <c r="D24" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="113"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="108"/>
+      <c r="E24" s="125"/>
+      <c r="F24" s="126"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="119"/>
+      <c r="I24" s="120"/>
       <c r="N24" s="11"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
@@ -2396,158 +2395,158 @@
         <v>17</v>
       </c>
       <c r="D25" s="65" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="115">
+        <v>99</v>
+      </c>
+      <c r="E25" s="106">
         <v>5000</v>
       </c>
-      <c r="F25" s="116"/>
-      <c r="G25" s="122"/>
-      <c r="H25" s="122"/>
-      <c r="I25" s="123"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="132"/>
+      <c r="H25" s="132"/>
+      <c r="I25" s="133"/>
       <c r="N25" s="11"/>
     </row>
     <row r="26" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="10"/>
-      <c r="C26" s="127" t="s">
+      <c r="C26" s="98" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="115">
+        <v>92</v>
+      </c>
+      <c r="E26" s="106">
         <v>3000</v>
       </c>
-      <c r="F26" s="116"/>
-      <c r="G26" s="105" t="s">
+      <c r="F26" s="107"/>
+      <c r="G26" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="105"/>
-      <c r="I26" s="106"/>
+      <c r="H26" s="117"/>
+      <c r="I26" s="118"/>
       <c r="N26" s="11"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
-      <c r="C27" s="128"/>
+      <c r="C27" s="99"/>
       <c r="D27" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="115">
+        <v>93</v>
+      </c>
+      <c r="E27" s="106">
         <v>1400</v>
       </c>
-      <c r="F27" s="116"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="106"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="118"/>
       <c r="N27" s="11"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
-      <c r="C28" s="128"/>
+      <c r="C28" s="99"/>
       <c r="D28" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="E28" s="115">
+        <v>94</v>
+      </c>
+      <c r="E28" s="106">
         <v>1630</v>
       </c>
-      <c r="F28" s="116"/>
-      <c r="G28" s="105"/>
-      <c r="H28" s="105"/>
-      <c r="I28" s="106"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="117"/>
+      <c r="I28" s="118"/>
       <c r="N28" s="11"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="10"/>
-      <c r="C29" s="128"/>
+      <c r="C29" s="99"/>
       <c r="D29" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="115">
+        <v>95</v>
+      </c>
+      <c r="E29" s="106">
         <v>3816</v>
       </c>
-      <c r="F29" s="116"/>
-      <c r="G29" s="105"/>
-      <c r="H29" s="105"/>
-      <c r="I29" s="106"/>
+      <c r="F29" s="107"/>
+      <c r="G29" s="117"/>
+      <c r="H29" s="117"/>
+      <c r="I29" s="118"/>
       <c r="N29" s="11"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
-      <c r="C30" s="128"/>
+      <c r="C30" s="99"/>
       <c r="D30" s="65" t="s">
-        <v>98</v>
-      </c>
-      <c r="E30" s="115">
+        <v>97</v>
+      </c>
+      <c r="E30" s="106">
         <v>1611</v>
       </c>
-      <c r="F30" s="116"/>
-      <c r="G30" s="105"/>
-      <c r="H30" s="105"/>
-      <c r="I30" s="106"/>
+      <c r="F30" s="107"/>
+      <c r="G30" s="117"/>
+      <c r="H30" s="117"/>
+      <c r="I30" s="118"/>
       <c r="N30" s="11"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="10"/>
-      <c r="C31" s="130"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="115">
+        <v>96</v>
+      </c>
+      <c r="E31" s="106">
         <v>8800</v>
       </c>
-      <c r="F31" s="116"/>
-      <c r="G31" s="105"/>
-      <c r="H31" s="105"/>
-      <c r="I31" s="106"/>
+      <c r="F31" s="107"/>
+      <c r="G31" s="117"/>
+      <c r="H31" s="117"/>
+      <c r="I31" s="118"/>
       <c r="N31" s="11"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
-      <c r="C32" s="127" t="s">
+      <c r="C32" s="98" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="65" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" s="115">
+        <v>98</v>
+      </c>
+      <c r="E32" s="106">
         <v>1250</v>
       </c>
-      <c r="F32" s="116"/>
-      <c r="G32" s="107" t="s">
+      <c r="F32" s="107"/>
+      <c r="G32" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="107"/>
-      <c r="I32" s="108"/>
+      <c r="H32" s="119"/>
+      <c r="I32" s="120"/>
       <c r="N32" s="11"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="10"/>
-      <c r="C33" s="128"/>
+      <c r="C33" s="99"/>
       <c r="D33" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="115">
+      <c r="E33" s="106">
         <v>45097</v>
       </c>
-      <c r="F33" s="116"/>
-      <c r="G33" s="107"/>
-      <c r="H33" s="107"/>
-      <c r="I33" s="108"/>
+      <c r="F33" s="107"/>
+      <c r="G33" s="119"/>
+      <c r="H33" s="119"/>
+      <c r="I33" s="120"/>
       <c r="N33" s="11"/>
     </row>
     <row r="34" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
-      <c r="C34" s="129"/>
+      <c r="C34" s="100"/>
       <c r="D34" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="134">
+      <c r="E34" s="108">
         <v>541164</v>
       </c>
-      <c r="F34" s="135"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="110"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="121"/>
+      <c r="H34" s="121"/>
+      <c r="I34" s="122"/>
       <c r="N34" s="11"/>
     </row>
     <row r="35" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2567,6 +2566,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G23:I24"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G32:I34"/>
+    <mergeCell ref="E23:F24"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="C26:C31"/>
@@ -2583,26 +2602,6 @@
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="C14:M14"/>
     <mergeCell ref="G26:I31"/>
-    <mergeCell ref="G32:I34"/>
-    <mergeCell ref="E23:F24"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G23:I24"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G16" r:id="rId1" xr:uid="{6C4BC0A4-2739-443E-9E0A-5FE4AD90A491}"/>
@@ -2620,8 +2619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4854C51-668C-46D5-A124-6BE70347F79A}">
   <dimension ref="B2:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="C1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2848,7 +2847,7 @@
         <v>7850</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K11" s="11"/>
     </row>

</xml_diff>